<commit_message>
Many changes, VaR, montecarlo, etc... dubject to change most probably
</commit_message>
<xml_diff>
--- a/portfolio-optimization/results/selected_assets_summary.xlsx
+++ b/portfolio-optimization/results/selected_assets_summary.xlsx
@@ -470,13 +470,13 @@
         <v>0.2</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04853781849854683</v>
+        <v>0.04879550243866605</v>
       </c>
       <c r="D2" t="n">
-        <v>0.005964918959102302</v>
+        <v>0.005954525361048833</v>
       </c>
       <c r="E2" t="n">
-        <v>1.59898542862722</v>
+        <v>1.645051762268533</v>
       </c>
     </row>
     <row r="3">
@@ -489,13 +489,13 @@
         <v>0.2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.185406672835213</v>
+        <v>0.1884369884805298</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1427643314286411</v>
+        <v>0.1427852673396272</v>
       </c>
       <c r="E3" t="n">
-        <v>1.025512965109163</v>
+        <v>1.046585486477964</v>
       </c>
     </row>
     <row r="4">
@@ -508,13 +508,13 @@
         <v>0.2</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1104650916466789</v>
+        <v>0.1177273822883147</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1103206053183034</v>
+        <v>0.1097642259820403</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6477945932265663</v>
+        <v>0.7172408094163223</v>
       </c>
     </row>
     <row r="5">
@@ -524,16 +524,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1926523418192495</v>
+        <v>0.1875320075471793</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1156351336166244</v>
+        <v>0.1197300911685313</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1144895806712278</v>
+        <v>0.1143798086650707</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6693633880684083</v>
+        <v>0.7058071884429076</v>
       </c>
     </row>
     <row r="6">
@@ -543,16 +543,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1525563661451452</v>
+        <v>0.152155804319207</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2180492408084803</v>
+        <v>0.2281010324356234</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2342863732530265</v>
+        <v>0.2338861163958089</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7642324148964019</v>
+        <v>0.8085175612373885</v>
       </c>
     </row>
     <row r="7">
@@ -562,16 +562,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.05479129202704688</v>
+        <v>0.06031218813333689</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1038370154838628</v>
+        <v>0.1090459691992094</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1482993988136657</v>
+        <v>0.1481662248229568</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4372034951087616</v>
+        <v>0.472752607977338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>